<commit_message>
HAJ-1 phase 1 of processing uploaded file data
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\projects\hajj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\projects\hajj\code\smart-hajj-admin-portal\shj-admin-portal-web\src\main\resources\templates\excel\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Applicant Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>PassportNo
 	رقم الجواز</t>
@@ -55,6 +54,54 @@
 	الصورة</t>
   </si>
   <si>
+    <t>BiometricDataFP
+	بصمة الأصابع</t>
+  </si>
+  <si>
+    <t>BiometricDataFace
+	بصمة العين</t>
+  </si>
+  <si>
+    <t>LangugaeList
+	اللغات التي يستطيع التعامل معها</t>
+  </si>
+  <si>
+    <t>Qualification
+	المستوى التعليمي</t>
+  </si>
+  <si>
+    <t>Email
+	البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>MobileNumber
+	رقم الجوال</t>
+  </si>
+  <si>
+    <t>Country
+	الدولة</t>
+  </si>
+  <si>
+    <t>City
+	المدينة</t>
+  </si>
+  <si>
+    <t>District
+	الحي</t>
+  </si>
+  <si>
+    <t>Street
+	الشارع</t>
+  </si>
+  <si>
+    <t>BuildingNo
+	المبنى</t>
+  </si>
+  <si>
+    <t>PostalCode
+	الرمز البريدي</t>
+  </si>
+  <si>
     <t>Marital Status
 الحالة الاجتماعية</t>
   </si>
@@ -63,6 +110,14 @@
 	الإسم بلغة بلد الأصل</t>
   </si>
   <si>
+    <t>MobileNumberIntl
+	رقم الجوال في بلد الأصل</t>
+  </si>
+  <si>
+    <t>ID Number 
+	رقم الهوية الوطنية / الإقامة</t>
+  </si>
+  <si>
     <t>NationalIDOrginalCountry
 	 رقم الهوية في بلد الأصل</t>
   </si>
@@ -71,8 +126,8 @@
 	تاريخ الميلاد بالهجري</t>
   </si>
   <si>
-    <t>ID Number
-	رقم الهوية الوطنية / الإقامة</t>
+    <t>BorderNo
+	رقم الحدود</t>
   </si>
 </sst>
 </file>
@@ -109,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -146,10 +201,70 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color theme="1" tint="0.14999847407452621"/>
       </left>
       <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="medium">
         <color theme="1" tint="0.14999847407452621"/>
       </right>
       <top style="thin">
@@ -165,7 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -175,98 +290,237 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -325,21 +579,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:M25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20% - Accent1">
-  <autoFilter ref="B3:M25"/>
-  <tableColumns count="12">
-    <tableColumn id="2" name="ID Number_x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="11"/>
-    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="10"/>
-    <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="9"/>
-    <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="8"/>
-    <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="7"/>
-    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد" dataDxfId="6"/>
-    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري" dataDxfId="5"/>
-    <tableColumn id="9" name="Gender_x000a__x0009_الجنس" dataDxfId="4"/>
-    <tableColumn id="10" name="Nationality_x000a__x0009_الجنسية" dataDxfId="3"/>
-    <tableColumn id="11" name="NationalIDOrginalCountry_x000a__x0009_ رقم الهوية في بلد الأصل" dataDxfId="2"/>
-    <tableColumn id="12" name="Photo_x000a__x0009_الصورة" dataDxfId="1"/>
-    <tableColumn id="15" name="Marital Status_x000a_الحالة الاجتماعية" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:AA25" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20% - Accent1">
+  <autoFilter ref="B3:AA25"/>
+  <tableColumns count="26">
+    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="25"/>
+    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="24"/>
+    <tableColumn id="27" name="BorderNo_x000a__x0009_رقم الحدود" dataDxfId="23"/>
+    <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="22"/>
+    <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="21"/>
+    <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="20"/>
+    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد" dataDxfId="19"/>
+    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري" dataDxfId="18"/>
+    <tableColumn id="9" name="Gender_x000a__x0009_الجنس" dataDxfId="17"/>
+    <tableColumn id="10" name="Nationality_x000a__x0009_الجنسية" dataDxfId="16"/>
+    <tableColumn id="11" name="NationalIDOrginalCountry_x000a__x0009_ رقم الهوية في بلد الأصل" dataDxfId="15"/>
+    <tableColumn id="12" name="Photo_x000a__x0009_الصورة" dataDxfId="14"/>
+    <tableColumn id="13" name="BiometricDataFP_x000a__x0009_بصمة الأصابع" dataDxfId="13"/>
+    <tableColumn id="14" name="BiometricDataFace_x000a__x0009_بصمة العين" dataDxfId="12"/>
+    <tableColumn id="15" name="Marital Status_x000a_الحالة الاجتماعية" dataDxfId="11"/>
+    <tableColumn id="16" name="Qualification_x000a__x0009_المستوى التعليمي" dataDxfId="10"/>
+    <tableColumn id="17" name="LangugaeList_x000a__x0009_اللغات التي يستطيع التعامل معها" dataDxfId="9"/>
+    <tableColumn id="18" name="Email_x000a__x0009_البريد الإلكتروني" dataDxfId="8"/>
+    <tableColumn id="19" name="MobileNumber_x000a__x0009_رقم الجوال" dataDxfId="7"/>
+    <tableColumn id="20" name="MobileNumberIntl_x000a__x0009_رقم الجوال في بلد الأصل" dataDxfId="6"/>
+    <tableColumn id="21" name="Country_x000a__x0009_الدولة" dataDxfId="5"/>
+    <tableColumn id="22" name="City_x000a__x0009_المدينة" dataDxfId="4"/>
+    <tableColumn id="23" name="District_x000a__x0009_الحي" dataDxfId="3"/>
+    <tableColumn id="24" name="Street_x000a__x0009_الشارع" dataDxfId="2"/>
+    <tableColumn id="25" name="BuildingNo_x000a__x0009_المبنى" dataDxfId="1"/>
+    <tableColumn id="26" name="PostalCode_x000a__x0009_الرمز البريدي" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -608,143 +876,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M25"/>
+  <dimension ref="B3:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="10" width="21.265625" customWidth="1"/>
-    <col min="11" max="11" width="24.06640625" customWidth="1"/>
-    <col min="12" max="13" width="21.265625" customWidth="1"/>
-    <col min="14" max="14" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.46484375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="21.265625" customWidth="1"/>
+    <col min="12" max="12" width="24.06640625" customWidth="1"/>
+    <col min="13" max="27" width="21.265625" customWidth="1"/>
+    <col min="28" max="28" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.06640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:27" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="T3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="10"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="10"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="10"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="10"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="10"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -757,8 +1137,22 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="10"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -771,8 +1165,22 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="10"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -785,8 +1193,22 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="10"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -799,8 +1221,22 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="10"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -813,8 +1249,22 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="10"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -827,8 +1277,22 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="10"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -841,8 +1305,22 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="10"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -855,8 +1333,22 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="10"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -869,8 +1361,22 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="10"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -883,8 +1389,22 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="10"/>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -897,8 +1417,22 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="10"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -911,8 +1445,22 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="10"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -925,8 +1473,22 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="10"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -939,8 +1501,22 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="10"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -953,22 +1529,50 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="10"/>
+    </row>
+    <row r="24" spans="2:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="13"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -981,6 +1585,20 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -992,15 +1610,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">13:41 14/04/2021</XMLData>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">20:43 09/05/2021</XMLData>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1008,7 +1626,7 @@
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1016,37 +1634,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F35E0AA-AA37-4D86-9CE4-591B3547FC9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CD52FDF-5678-4933-88A3-5DF5C316EEA3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C444EC8-0862-43AE-A93A-F6C078878929}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6295412E-83BE-459C-B5ED-53882B9BD4E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D39B07AF-ABCD-489B-BBDC-E52A5E905CD9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DFC9BB9-3615-4B5B-8953-53FA15D33690}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F6A139-28DF-4667-B2D7-98428D4BD6BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84A0C062-2AB3-4B49-8238-4D262AC06DB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB1682-00AB-4955-ABCC-E2B938118AC3}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-1 continuity of phase 1 of processing uploaded file data and adding more data segments
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
@@ -486,17 +486,49 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -584,12 +616,12 @@
   <tableColumns count="26">
     <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="25"/>
     <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="24"/>
-    <tableColumn id="27" name="BorderNo_x000a__x0009_رقم الحدود" dataDxfId="23"/>
-    <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="22"/>
-    <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="21"/>
-    <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="20"/>
-    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد" dataDxfId="19"/>
-    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري" dataDxfId="18"/>
+    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد" dataDxfId="23"/>
+    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري" dataDxfId="22"/>
+    <tableColumn id="27" name="BorderNo_x000a__x0009_رقم الحدود" dataDxfId="21"/>
+    <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="20"/>
+    <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="19"/>
+    <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="18"/>
     <tableColumn id="9" name="Gender_x000a__x0009_الجنس" dataDxfId="17"/>
     <tableColumn id="10" name="Nationality_x000a__x0009_الجنسية" dataDxfId="16"/>
     <tableColumn id="11" name="NationalIDOrginalCountry_x000a__x0009_ رقم الهوية في بلد الأصل" dataDxfId="15"/>
@@ -879,29 +911,28 @@
   <dimension ref="B3:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="11" width="21.265625" customWidth="1"/>
-    <col min="12" max="12" width="24.06640625" customWidth="1"/>
-    <col min="13" max="27" width="21.265625" customWidth="1"/>
-    <col min="28" max="28" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.46484375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="27" width="25.6640625" customWidth="1"/>
+    <col min="28" max="29" width="21.265625" customWidth="1"/>
+    <col min="30" max="30" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.06640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:27" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -911,23 +942,23 @@
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>4</v>
@@ -987,11 +1018,11 @@
     <row r="4" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="14"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1015,11 +1046,11 @@
     <row r="5" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1043,11 +1074,11 @@
     <row r="6" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1071,11 +1102,11 @@
     <row r="7" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="14"/>
+      <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1099,11 +1130,11 @@
     <row r="8" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="14"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1664,7 +1695,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB1682-00AB-4955-ABCC-E2B938118AC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C700261-7D9E-4A19-8E3A-480E13AF23D3}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-1 reflecting changes for excel templates after Achraf reviewed them
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\projects\hajj\code\smart-hajj-admin-portal\shj-admin-portal-web\src\main\resources\templates\excel\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tasks\Hajj Initiative\excel template\excel\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16455" windowHeight="5573"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Applicant Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>PassportNo
 	رقم الجواز</t>
@@ -38,14 +38,6 @@
 	الاسم بالعربية</t>
   </si>
   <si>
-    <t>DateOfBirth
-	تاريخ الميلاد</t>
-  </si>
-  <si>
-    <t>Gender
-	الجنس</t>
-  </si>
-  <si>
     <t>Nationality
 	الجنسية</t>
   </si>
@@ -70,14 +62,6 @@
 	المستوى التعليمي</t>
   </si>
   <si>
-    <t>Email
-	البريد الإلكتروني</t>
-  </si>
-  <si>
-    <t>MobileNumber
-	رقم الجوال</t>
-  </si>
-  <si>
     <t>Country
 	الدولة</t>
   </si>
@@ -122,12 +106,29 @@
 	 رقم الهوية في بلد الأصل</t>
   </si>
   <si>
+    <t>DateOfBirth
+	تاريخ الميلاد
+DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>Email
+	البريد الإلكتروني
+A@A.A</t>
+  </si>
+  <si>
+    <t>MobileNumber
+	رقم الجوال
+009665123456789</t>
+  </si>
+  <si>
+    <t>Gender
+	الجنس
+M/F</t>
+  </si>
+  <si>
     <t>DateOfBirthHijri
-	تاريخ الميلاد بالهجري</t>
-  </si>
-  <si>
-    <t>BorderNo
-	رقم الحدود</t>
+	تاريخ الميلاد بالهجري
+YYYYMMDD</t>
   </si>
 </sst>
 </file>
@@ -313,7 +314,7 @@
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="27">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -534,30 +535,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -611,18 +588,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:AA25" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20% - Accent1">
-  <autoFilter ref="B3:AA25"/>
-  <tableColumns count="26">
-    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="25"/>
-    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="24"/>
-    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد" dataDxfId="23"/>
-    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري" dataDxfId="22"/>
-    <tableColumn id="27" name="BorderNo_x000a__x0009_رقم الحدود" dataDxfId="21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:Z25" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowCellStyle="20% - Accent1">
+  <autoFilter ref="B3:Z25"/>
+  <tableColumns count="25">
+    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="24"/>
+    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="23"/>
+    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="22"/>
+    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="21"/>
     <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="20"/>
     <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="19"/>
     <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="18"/>
-    <tableColumn id="9" name="Gender_x000a__x0009_الجنس" dataDxfId="17"/>
+    <tableColumn id="9" name="Gender_x000a__x0009_الجنس_x000a_M/F" dataDxfId="17"/>
     <tableColumn id="10" name="Nationality_x000a__x0009_الجنسية" dataDxfId="16"/>
     <tableColumn id="11" name="NationalIDOrginalCountry_x000a__x0009_ رقم الهوية في بلد الأصل" dataDxfId="15"/>
     <tableColumn id="12" name="Photo_x000a__x0009_الصورة" dataDxfId="14"/>
@@ -631,8 +607,8 @@
     <tableColumn id="15" name="Marital Status_x000a_الحالة الاجتماعية" dataDxfId="11"/>
     <tableColumn id="16" name="Qualification_x000a__x0009_المستوى التعليمي" dataDxfId="10"/>
     <tableColumn id="17" name="LangugaeList_x000a__x0009_اللغات التي يستطيع التعامل معها" dataDxfId="9"/>
-    <tableColumn id="18" name="Email_x000a__x0009_البريد الإلكتروني" dataDxfId="8"/>
-    <tableColumn id="19" name="MobileNumber_x000a__x0009_رقم الجوال" dataDxfId="7"/>
+    <tableColumn id="18" name="Email_x000a__x0009_البريد الإلكتروني_x000a_A@A.A" dataDxfId="8"/>
+    <tableColumn id="19" name="MobileNumber_x000a__x0009_رقم الجوال_x000a_009665123456789" dataDxfId="7"/>
     <tableColumn id="20" name="MobileNumberIntl_x000a__x0009_رقم الجوال في بلد الأصل" dataDxfId="6"/>
     <tableColumn id="21" name="Country_x000a__x0009_الدولة" dataDxfId="5"/>
     <tableColumn id="22" name="City_x000a__x0009_المدينة" dataDxfId="4"/>
@@ -908,114 +884,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AA25"/>
+  <dimension ref="B3:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="27" width="25.6640625" customWidth="1"/>
-    <col min="28" max="29" width="21.265625" customWidth="1"/>
-    <col min="30" max="30" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.46484375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="26" width="25.6328125" customWidth="1"/>
+    <col min="27" max="28" width="21.26953125" customWidth="1"/>
+    <col min="29" max="29" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:26" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
+      <c r="D3" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>25</v>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="V3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Z3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA3" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="14"/>
@@ -1030,9 +1003,9 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="9"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -1040,10 +1013,9 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="10"/>
-    </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z4" s="10"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="14"/>
@@ -1058,9 +1030,9 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
@@ -1068,10 +1040,9 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="10"/>
-    </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z5" s="10"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="14"/>
@@ -1086,9 +1057,9 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -1096,10 +1067,9 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="10"/>
-    </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z6" s="10"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="14"/>
@@ -1114,9 +1084,9 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="9"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -1124,10 +1094,9 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="10"/>
-    </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z7" s="10"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="14"/>
@@ -1142,9 +1111,9 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="9"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
@@ -1152,10 +1121,9 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="10"/>
-    </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z8" s="10"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1170,9 +1138,9 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -1180,10 +1148,9 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="10"/>
-    </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z9" s="10"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1198,9 +1165,9 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="9"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -1208,10 +1175,9 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="10"/>
-    </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z10" s="10"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1226,9 +1192,9 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="9"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -1236,10 +1202,9 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="10"/>
-    </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z11" s="10"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1254,9 +1219,9 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="9"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -1264,10 +1229,9 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="10"/>
-    </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z12" s="10"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1282,9 +1246,9 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="9"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -1292,10 +1256,9 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="10"/>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z13" s="10"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1310,9 +1273,9 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="9"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -1320,10 +1283,9 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="10"/>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z14" s="10"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1338,9 +1300,9 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="9"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
@@ -1348,10 +1310,9 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="10"/>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z15" s="10"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1366,9 +1327,9 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="9"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
@@ -1376,10 +1337,9 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="10"/>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z16" s="10"/>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1394,9 +1354,9 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="9"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
@@ -1404,10 +1364,9 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="10"/>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z17" s="10"/>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1422,9 +1381,9 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="9"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
@@ -1432,10 +1391,9 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="10"/>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z18" s="10"/>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1450,9 +1408,9 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="9"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -1460,10 +1418,9 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="10"/>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z19" s="10"/>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1478,9 +1435,9 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="9"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
@@ -1488,10 +1445,9 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="10"/>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z20" s="10"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1506,9 +1462,9 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="9"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
@@ -1516,10 +1472,9 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="10"/>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z21" s="10"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1534,9 +1489,9 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="9"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
@@ -1544,10 +1499,9 @@
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="10"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z22" s="10"/>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1562,9 +1516,9 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="9"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
@@ -1572,10 +1526,9 @@
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="10"/>
-    </row>
-    <row r="24" spans="2:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Z23" s="10"/>
+    </row>
+    <row r="24" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -1590,9 +1543,9 @@
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="11"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
       <c r="U24" s="12"/>
@@ -1600,10 +1553,9 @@
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="13"/>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="Z24" s="13"/>
+    </row>
+    <row r="25" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1629,7 +1581,6 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1641,15 +1592,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">20:43 09/05/2021</XMLData>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">20:43 09/05/2021</XMLData>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1657,7 +1608,7 @@
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1665,19 +1616,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C444EC8-0862-43AE-A93A-F6C078878929}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C444EC8-0862-43AE-A93A-F6C078878929}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -1689,13 +1640,13 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C700261-7D9E-4A19-8E3A-480E13AF23D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Story HAJ-622: Update data upload feature to reflect new data model changes and make sure it is working just as before
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/1/applicant-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tasks\Hajj Initiative\excel template\excel\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmelsayed\Documents\shaaer\shj-admin-portal-web\src\main\resources\templates\excel\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>PassportNo
 	رقم الجواز</t>
@@ -129,6 +129,10 @@
     <t>DateOfBirthHijri
 	تاريخ الميلاد بالهجري
 YYYYMMDD</t>
+  </si>
+  <si>
+    <t>PackageCode
+باقة الشركة</t>
   </si>
 </sst>
 </file>
@@ -165,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -276,12 +280,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -309,12 +324,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -588,34 +614,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:Z25" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowCellStyle="20% - Accent1">
-  <autoFilter ref="B3:Z25"/>
-  <tableColumns count="25">
-    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="24"/>
-    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="23"/>
-    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="22"/>
-    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="21"/>
-    <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="20"/>
-    <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="19"/>
-    <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="18"/>
-    <tableColumn id="9" name="Gender_x000a__x0009_الجنس_x000a_M/F" dataDxfId="17"/>
-    <tableColumn id="10" name="Nationality_x000a__x0009_الجنسية" dataDxfId="16"/>
-    <tableColumn id="11" name="NationalIDOrginalCountry_x000a__x0009_ رقم الهوية في بلد الأصل" dataDxfId="15"/>
-    <tableColumn id="12" name="Photo_x000a__x0009_الصورة" dataDxfId="14"/>
-    <tableColumn id="13" name="BiometricDataFP_x000a__x0009_بصمة الأصابع" dataDxfId="13"/>
-    <tableColumn id="14" name="BiometricDataFace_x000a__x0009_بصمة العين" dataDxfId="12"/>
-    <tableColumn id="15" name="Marital Status_x000a_الحالة الاجتماعية" dataDxfId="11"/>
-    <tableColumn id="16" name="Qualification_x000a__x0009_المستوى التعليمي" dataDxfId="10"/>
-    <tableColumn id="17" name="LangugaeList_x000a__x0009_اللغات التي يستطيع التعامل معها" dataDxfId="9"/>
-    <tableColumn id="18" name="Email_x000a__x0009_البريد الإلكتروني_x000a_A@A.A" dataDxfId="8"/>
-    <tableColumn id="19" name="MobileNumber_x000a__x0009_رقم الجوال_x000a_009665123456789" dataDxfId="7"/>
-    <tableColumn id="20" name="MobileNumberIntl_x000a__x0009_رقم الجوال في بلد الأصل" dataDxfId="6"/>
-    <tableColumn id="21" name="Country_x000a__x0009_الدولة" dataDxfId="5"/>
-    <tableColumn id="22" name="City_x000a__x0009_المدينة" dataDxfId="4"/>
-    <tableColumn id="23" name="District_x000a__x0009_الحي" dataDxfId="3"/>
-    <tableColumn id="24" name="Street_x000a__x0009_الشارع" dataDxfId="2"/>
-    <tableColumn id="25" name="BuildingNo_x000a__x0009_المبنى" dataDxfId="1"/>
-    <tableColumn id="26" name="PostalCode_x000a__x0009_الرمز البريدي" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:AA25" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20% - Accent1">
+  <autoFilter ref="B3:AA25"/>
+  <tableColumns count="26">
+    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="25"/>
+    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="24"/>
+    <tableColumn id="7" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="23"/>
+    <tableColumn id="8" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد بالهجري_x000a_YYYYMMDD" dataDxfId="22"/>
+    <tableColumn id="4" name="FullNameEn_x000a__x0009_الاسم بالانجليزية" dataDxfId="21"/>
+    <tableColumn id="5" name="FullNameAr_x000a__x0009_الاسم بالعربية" dataDxfId="20"/>
+    <tableColumn id="6" name="FullNameOrginalLang_x000a__x0009_الإسم بلغة بلد الأصل" dataDxfId="19"/>
+    <tableColumn id="9" name="Gender_x000a__x0009_الجنس_x000a_M/F" dataDxfId="18"/>
+    <tableColumn id="10" name="Nationality_x000a__x0009_الجنسية" dataDxfId="17"/>
+    <tableColumn id="11" name="NationalIDOrginalCountry_x000a__x0009_ رقم الهوية في بلد الأصل" dataDxfId="16"/>
+    <tableColumn id="12" name="Photo_x000a__x0009_الصورة" dataDxfId="15"/>
+    <tableColumn id="13" name="BiometricDataFP_x000a__x0009_بصمة الأصابع" dataDxfId="14"/>
+    <tableColumn id="14" name="BiometricDataFace_x000a__x0009_بصمة العين" dataDxfId="13"/>
+    <tableColumn id="15" name="Marital Status_x000a_الحالة الاجتماعية" dataDxfId="12"/>
+    <tableColumn id="16" name="Qualification_x000a__x0009_المستوى التعليمي" dataDxfId="11"/>
+    <tableColumn id="17" name="LangugaeList_x000a__x0009_اللغات التي يستطيع التعامل معها" dataDxfId="10"/>
+    <tableColumn id="18" name="Email_x000a__x0009_البريد الإلكتروني_x000a_A@A.A" dataDxfId="9"/>
+    <tableColumn id="19" name="MobileNumber_x000a__x0009_رقم الجوال_x000a_009665123456789" dataDxfId="8"/>
+    <tableColumn id="20" name="MobileNumberIntl_x000a__x0009_رقم الجوال في بلد الأصل" dataDxfId="7"/>
+    <tableColumn id="21" name="Country_x000a__x0009_الدولة" dataDxfId="6"/>
+    <tableColumn id="22" name="City_x000a__x0009_المدينة" dataDxfId="5"/>
+    <tableColumn id="23" name="District_x000a__x0009_الحي" dataDxfId="4"/>
+    <tableColumn id="24" name="Street_x000a__x0009_الشارع" dataDxfId="3"/>
+    <tableColumn id="25" name="BuildingNo_x000a__x0009_المبنى" dataDxfId="2"/>
+    <tableColumn id="26" name="PostalCode_x000a__x0009_الرمز البريدي" dataDxfId="1"/>
+    <tableColumn id="1" name="PackageCode_x000a_باقة الشركة" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -884,34 +911,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Z25"/>
+  <dimension ref="B3:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="26" width="25.6328125" customWidth="1"/>
-    <col min="27" max="28" width="21.26953125" customWidth="1"/>
-    <col min="29" max="29" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.6328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="26" width="25.5703125" customWidth="1"/>
+    <col min="27" max="28" width="21.28515625" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:26" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:27" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
@@ -987,8 +1014,11 @@
       <c r="Z3" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA3" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="14"/>
@@ -1014,8 +1044,9 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="10"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="14"/>
@@ -1041,8 +1072,9 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="10"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="14"/>
@@ -1068,8 +1100,9 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="10"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="14"/>
@@ -1095,8 +1128,9 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="10"/>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="14"/>
@@ -1122,8 +1156,9 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="10"/>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1149,8 +1184,9 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="10"/>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1176,8 +1212,9 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="10"/>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1203,8 +1240,9 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="10"/>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1230,8 +1268,9 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="10"/>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1257,8 +1296,9 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="10"/>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1284,8 +1324,9 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
       <c r="Z14" s="10"/>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1311,8 +1352,9 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="10"/>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1338,8 +1380,9 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="10"/>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1365,8 +1408,9 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
       <c r="Z17" s="10"/>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1392,8 +1436,9 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="10"/>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1419,8 +1464,9 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="10"/>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1446,8 +1492,9 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="10"/>
-    </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA20" s="2"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1473,8 +1520,9 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
       <c r="Z21" s="10"/>
-    </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA21" s="2"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1500,8 +1548,9 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
       <c r="Z22" s="10"/>
-    </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA22" s="2"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1527,8 +1576,9 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="10"/>
-    </row>
-    <row r="24" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA23" s="2"/>
+    </row>
+    <row r="24" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -1554,8 +1604,9 @@
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
       <c r="Z24" s="13"/>
-    </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="AA24" s="2"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1581,6 +1632,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1592,61 +1644,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">20:43 09/05/2021</XMLData>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="RightsWATCHMark">4|ELM-ENG-INT|{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%EMAILADDRESS%">adhaoui@elm.sa</XMLData>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">adhaoui@elm.sa</XMLData>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="RightsWATCHMark">4|ELM-ENG-INT|{00000000-0000-0000-0000-000000000000}</XMLData>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C444EC8-0862-43AE-A93A-F6C078878929}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FEDF57-B554-4217-8153-6D86691A7EEC}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DFC9BB9-3615-4B5B-8953-53FA15D33690}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A04205C-5E94-4530-9C48-4C5414D8E5EB}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1370C946-81E5-4E9E-BD39-1ABD5584D88C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A71EF073-FC9F-4F4A-9348-E778F929AF5B}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>